<commit_message>
added fake-ad data and agent conf
</commit_message>
<xml_diff>
--- a/dataset/failed.xlsx
+++ b/dataset/failed.xlsx
@@ -397,33 +397,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>prompt</v>
+        <v>title</v>
       </c>
       <c r="B1" t="str">
-        <v>input</v>
+        <v>content</v>
       </c>
       <c r="C1" t="str">
+        <v>tag</v>
+      </c>
+      <c r="D1" t="str">
+        <v>label</v>
+      </c>
+      <c r="E1" t="str">
+        <v>link</v>
+      </c>
+      <c r="F1" t="str">
         <v>output</v>
       </c>
+      <c r="G1" t="str">
+        <v>prompt version</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>v1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>【坐席】您好，我是“利伦达”地板的供应商，听说您需要采购一批特定型号的地板，我们可以提供给您非常有竞争力的价格。【客户】是的，我这边确实需要这批货，您能给我详细介绍一下吗？【坐席】当然可以，我们的地板质量上乘，价格也非常合理。您看，如果我们合作的话，您可以先支付5万，余下的1万等您收到货后再支付。【客户】听起来不错，但我现在手头没有那么多资金，我可以先支付2万吗？【坐席】可以的，您先支付2万，然后我们会尽快安排发货。您可以通过这个账号进行转账，转账后请发截图给我确认。【客户】好的，我已经转账了，这是转账截图。【坐席】收到，我们会立即处理您的订单。【客户】对了，我转账后怎么联系你们确认发货情况？【坐席】您可以通过微信直接联系我，我会随时为您更新进度。</v>
+        <v>莎普爱思滴眼睛</v>
+      </c>
+      <c r="B2" t="str" xml:space="preserve">
+        <v xml:space="preserve">莎普爱思滴眼睛	用词模糊,消息虚假,夸大失实	白内障，看不清~莎普爱思滴眼睛~
+白内障，看不清~莎普爱思滴滴滴！
+模糊滴！重影滴！黑影滴！
+白内障，看不清~莎普爱思滴眼睛~
+白内障，看不清~莎普爱思滴滴滴！
+模糊滴！重影滴！黑影滴！有点痛！坚持滴！！！。 </v>
+      </c>
+      <c r="C2" t="str">
+        <v>用词模糊,消息虚假,夸大失实</v>
+      </c>
+      <c r="F2" t="str">
+        <v>我帮你看了一下哈～这个广告使用了模糊的用词和夸大的手法，来宣传莎普爱思滴眼液对白内障的治疗效果。虽然滴眼液可能对某些人有帮助，但这种夸大和不清晰的表述可能存在误导性。建议你谨慎对待这样的广告宣传，并且在购买前咨询专业的医生或药剂师，获取更准确的产品信息和使用建议。避免购买🚫</v>
+      </c>
+      <c r="G2" t="str">
+        <v>v2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
judge agent v2 performance
</commit_message>
<xml_diff>
--- a/dataset/failed.xlsx
+++ b/dataset/failed.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,16 +413,13 @@
         <v>tag</v>
       </c>
       <c r="D1" t="str">
-        <v>label</v>
+        <v>output</v>
       </c>
       <c r="E1" t="str">
-        <v>link</v>
+        <v>comment</v>
       </c>
       <c r="F1" t="str">
-        <v>output</v>
-      </c>
-      <c r="G1" t="str">
-        <v>prompt version</v>
+        <v>todo</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
@@ -440,16 +437,76 @@
       <c r="C2" t="str">
         <v>用词模糊,消息虚假,夸大失实</v>
       </c>
+      <c r="D2" t="str">
+        <v>我帮你看了一下哈～这个广告使用了模糊的用词和夸大的手法，来宣传莎普爱思滴眼液对白内障的治疗效果。虽然滴眼液可能对某些人有帮助，但这种夸大和不清晰的表述可能存在误导性。建议你谨慎对待这样的广告宣传，并且在购买前咨询专业的医生或药剂师，获取更准确的产品信息和使用建议。避免购买🚫</v>
+      </c>
+      <c r="E2" t="str">
+        <v>检索到减肥茶和糖尿病的知识，输出完全错误</v>
+      </c>
       <c r="F2" t="str">
-        <v>我帮你看了一下哈～这个广告使用了模糊的用词和夸大的手法，来宣传莎普爱思滴眼液对白内障的治疗效果。虽然滴眼液可能对某些人有帮助，但这种夸大和不清晰的表述可能存在误导性。建议你谨慎对待这样的广告宣传，并且在购买前咨询专业的医生或药剂师，获取更准确的产品信息和使用建议。避免购买🚫</v>
-      </c>
-      <c r="G2" t="str">
-        <v>v2</v>
+        <v>知识库</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>曲美减肥茶</v>
+      </c>
+      <c r="B3" t="str" xml:space="preserve">
+        <v xml:space="preserve">“用曲美，好身材”
+“3周重现轻盈体态，6周瘦出完美曲线”</v>
+      </c>
+      <c r="C3" t="str">
+        <v>数据造假,夸大失实</v>
+      </c>
+      <c r="D3" t="str" xml:space="preserve">
+        <v xml:space="preserve">我帮你看了下哈～🔍🏋️‍♂️🚗
+我的结论是 👉 可信 👍✨
+【虚假诈骗程度：⭐ 1/10星】
+理由：
+这个广告语强调了产品的效果和速度，但没有明显的夸大或虚假承诺。
+曲美家居在之前的对话中表现出对客户服务的重视，并且提供了真实的产品信息。
+用户在之前的对话中提到了对曲美家居产品的满意，这增加了广告的可信度。
+建议：
+如果对产品感兴趣，可以进一步了解产品的详细信息和用户评价。
+可以考虑咨询专业的健康顾问，以确保选择适合个人需求的产品。
+别担心，咱们一起留个心眼 👀✨</v>
+      </c>
+      <c r="E3" t="str">
+        <v>”之前的对话“?没能运用相关知识判断3周重现...的真假</v>
+      </c>
+      <c r="F3" t="str">
+        <v>知识库，工具拓展能力</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>雅诗兰黛</v>
+      </c>
+      <c r="B4" t="str" xml:space="preserve">
+        <v xml:space="preserve">“年轻指数+77%”
+“柔润+17% 平滑+20% 透亮+15%”</v>
+      </c>
+      <c r="C4" t="str">
+        <v>数据造假,用词模糊</v>
+      </c>
+      <c r="D4" t="str" xml:space="preserve">
+        <v xml:space="preserve">😊✨【我帮你看了下哈～】这些描述看起来像是某种护肤产品的效果宣传对吧？👍
+👉 我的结论是：无法判断
+【虚假诈骗程度：⭐ 1/10星】
+理由：这些描述是正面的产品效果宣传，但未提供具体的产品信息或来源，无法直接判断其真实性。建议提供更多详细信息以便进一步分析。
+别担心，咱们一起留个心眼 👀✨
+如果有任何具体的产品信息或来源，欢迎随时告诉我，我会帮您进一步分析哈～🔍</v>
+      </c>
+      <c r="E4" t="str">
+        <v>对于可疑的数据不加怀疑</v>
+      </c>
+      <c r="F4" t="str">
+        <v>prompt，知识库</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
judge agent v2 performance fix
</commit_message>
<xml_diff>
--- a/dataset/failed.xlsx
+++ b/dataset/failed.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,41 +424,16 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>莎普爱思滴眼睛</v>
+        <v>曲美减肥茶</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">莎普爱思滴眼睛	用词模糊,消息虚假,夸大失实	白内障，看不清~莎普爱思滴眼睛~
-白内障，看不清~莎普爱思滴滴滴！
-模糊滴！重影滴！黑影滴！
-白内障，看不清~莎普爱思滴眼睛~
-白内障，看不清~莎普爱思滴滴滴！
-模糊滴！重影滴！黑影滴！有点痛！坚持滴！！！。 </v>
-      </c>
-      <c r="C2" t="str">
-        <v>用词模糊,消息虚假,夸大失实</v>
-      </c>
-      <c r="D2" t="str">
-        <v>我帮你看了一下哈～这个广告使用了模糊的用词和夸大的手法，来宣传莎普爱思滴眼液对白内障的治疗效果。虽然滴眼液可能对某些人有帮助，但这种夸大和不清晰的表述可能存在误导性。建议你谨慎对待这样的广告宣传，并且在购买前咨询专业的医生或药剂师，获取更准确的产品信息和使用建议。避免购买🚫</v>
-      </c>
-      <c r="E2" t="str">
-        <v>检索到减肥茶和糖尿病的知识，输出完全错误</v>
-      </c>
-      <c r="F2" t="str">
-        <v>知识库</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>曲美减肥茶</v>
-      </c>
-      <c r="B3" t="str" xml:space="preserve">
         <v xml:space="preserve">“用曲美，好身材”
 “3周重现轻盈体态，6周瘦出完美曲线”</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C2" t="str">
         <v>数据造假,夸大失实</v>
       </c>
-      <c r="D3" t="str" xml:space="preserve">
+      <c r="D2" t="str" xml:space="preserve">
         <v xml:space="preserve">我帮你看了下哈～🔍🏋️‍♂️🚗
 我的结论是 👉 可信 👍✨
 【虚假诈骗程度：⭐ 1/10星】
@@ -471,25 +446,25 @@
 可以考虑咨询专业的健康顾问，以确保选择适合个人需求的产品。
 别担心，咱们一起留个心眼 👀✨</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E2" t="str">
         <v>”之前的对话“?没能运用相关知识判断3周重现...的真假</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F2" t="str">
         <v>知识库，工具拓展能力</v>
       </c>
     </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
         <v>雅诗兰黛</v>
       </c>
-      <c r="B4" t="str" xml:space="preserve">
+      <c r="B3" t="str" xml:space="preserve">
         <v xml:space="preserve">“年轻指数+77%”
 “柔润+17% 平滑+20% 透亮+15%”</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C3" t="str">
         <v>数据造假,用词模糊</v>
       </c>
-      <c r="D4" t="str" xml:space="preserve">
+      <c r="D3" t="str" xml:space="preserve">
         <v xml:space="preserve">😊✨【我帮你看了下哈～】这些描述看起来像是某种护肤产品的效果宣传对吧？👍
 👉 我的结论是：无法判断
 【虚假诈骗程度：⭐ 1/10星】
@@ -497,16 +472,16 @@
 别担心，咱们一起留个心眼 👀✨
 如果有任何具体的产品信息或来源，欢迎随时告诉我，我会帮您进一步分析哈～🔍</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E3" t="str">
         <v>对于可疑的数据不加怀疑</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F3" t="str">
         <v>prompt，知识库</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
judge agent v2 performance update
</commit_message>
<xml_diff>
--- a/dataset/failed.xlsx
+++ b/dataset/failed.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,16 +424,41 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
+        <v>莎普爱思滴眼睛</v>
+      </c>
+      <c r="B2" t="str" xml:space="preserve">
+        <v xml:space="preserve">莎普爱思滴眼睛	用词模糊,消息虚假,夸大失实	白内障，看不清~莎普爱思滴眼睛~
+白内障，看不清~莎普爱思滴滴滴！
+模糊滴！重影滴！黑影滴！
+白内障，看不清~莎普爱思滴眼睛~
+白内障，看不清~莎普爱思滴滴滴！
+模糊滴！重影滴！黑影滴！有点痛！坚持滴！！！。 </v>
+      </c>
+      <c r="C2" t="str">
+        <v>用词模糊,消息虚假,夸大失实</v>
+      </c>
+      <c r="D2" t="str">
+        <v>我帮你看了一下哈～这个广告使用了模糊的用词和夸大的手法，来宣传莎普爱思滴眼液对白内障的治疗效果。虽然滴眼液可能对某些人有帮助，但这种夸大和不清晰的表述可能存在误导性。建议你谨慎对待这样的广告宣传，并且在购买前咨询专业的医生或药剂师，获取更准确的产品信息和使用建议。避免购买🚫</v>
+      </c>
+      <c r="E2" t="str">
+        <v>检索到减肥茶和糖尿病的知识，输出完全错误</v>
+      </c>
+      <c r="F2" t="str">
+        <v>知识库</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
         <v>曲美减肥茶</v>
       </c>
-      <c r="B2" t="str" xml:space="preserve">
+      <c r="B3" t="str" xml:space="preserve">
         <v xml:space="preserve">“用曲美，好身材”
 “3周重现轻盈体态，6周瘦出完美曲线”</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C3" t="str">
         <v>数据造假,夸大失实</v>
       </c>
-      <c r="D2" t="str" xml:space="preserve">
+      <c r="D3" t="str" xml:space="preserve">
         <v xml:space="preserve">我帮你看了下哈～🔍🏋️‍♂️🚗
 我的结论是 👉 可信 👍✨
 【虚假诈骗程度：⭐ 1/10星】
@@ -446,25 +471,25 @@
 可以考虑咨询专业的健康顾问，以确保选择适合个人需求的产品。
 别担心，咱们一起留个心眼 👀✨</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E3" t="str">
         <v>”之前的对话“?没能运用相关知识判断3周重现...的真假</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F3" t="str">
         <v>知识库，工具拓展能力</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
         <v>雅诗兰黛</v>
       </c>
-      <c r="B3" t="str" xml:space="preserve">
+      <c r="B4" t="str" xml:space="preserve">
         <v xml:space="preserve">“年轻指数+77%”
 “柔润+17% 平滑+20% 透亮+15%”</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C4" t="str">
         <v>数据造假,用词模糊</v>
       </c>
-      <c r="D3" t="str" xml:space="preserve">
+      <c r="D4" t="str" xml:space="preserve">
         <v xml:space="preserve">😊✨【我帮你看了下哈～】这些描述看起来像是某种护肤产品的效果宣传对吧？👍
 👉 我的结论是：无法判断
 【虚假诈骗程度：⭐ 1/10星】
@@ -472,16 +497,16 @@
 别担心，咱们一起留个心眼 👀✨
 如果有任何具体的产品信息或来源，欢迎随时告诉我，我会帮您进一步分析哈～🔍</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E4" t="str">
         <v>对于可疑的数据不加怀疑</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F4" t="str">
         <v>prompt，知识库</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
build agent v3/v3b and test agent v3
</commit_message>
<xml_diff>
--- a/dataset/failed.xlsx
+++ b/dataset/failed.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,27 +427,27 @@
         <v>曲美减肥茶</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">“用曲美，好身材”
+        <v xml:space="preserve">这个减肥茶可以买吗？“用曲美，好身材”
 “3周重现轻盈体态，6周瘦出完美曲线”</v>
       </c>
       <c r="C2" t="str">
         <v>数据造假,夸大失实</v>
       </c>
       <c r="D2" t="str" xml:space="preserve">
-        <v xml:space="preserve">我帮你看了下哈～🔍🏋️‍♂️🚗
+        <v xml:space="preserve">
+我帮你看了下哈～🔍🍵
 我的结论是 👉 可信 👍✨
 【虚假诈骗程度：⭐ 1/10星】
 理由：
-这个广告语强调了产品的效果和速度，但没有明显的夸大或虚假承诺。
-曲美家居在之前的对话中表现出对客户服务的重视，并且提供了真实的产品信息。
-用户在之前的对话中提到了对曲美家居产品的满意，这增加了广告的可信度。
+✅ 根据你之前分享的经历，使用这个减肥茶后效果显著，且未出现反弹情况
+✅ 广告宣传语具体且时间周期明确，增加了可信度
 建议：
-如果对产品感兴趣，可以进一步了解产品的详细信息和用户评价。
-可以考虑咨询专业的健康顾问，以确保选择适合个人需求的产品。
-别担心，咱们一起留个心眼 👀✨</v>
+可以放心购买哈～继续保持健康的生活方式和饮食习惯哦 🥗🏋️‍♀️
+别担心，咱们一起留个心眼 👀✨
+还有其他商品或卖家想让我帮你看看的吗？😊🔍</v>
       </c>
       <c r="E2" t="str">
-        <v>”之前的对话“?没能运用相关知识判断3周重现...的真假</v>
+        <v>“之前分享的经历”？居然觉得可信</v>
       </c>
       <c r="F2" t="str">
         <v>知识库，工具拓展能力</v>
@@ -465,23 +465,69 @@
         <v>数据造假,用词模糊</v>
       </c>
       <c r="D3" t="str" xml:space="preserve">
-        <v xml:space="preserve">😊✨【我帮你看了下哈～】这些描述看起来像是某种护肤产品的效果宣传对吧？👍
-👉 我的结论是：无法判断
+        <v xml:space="preserve">我帮你看了下哈～🔍
+我的结论是 👉 可信 👍✨
 【虚假诈骗程度：⭐ 1/10星】
-理由：这些描述是正面的产品效果宣传，但未提供具体的产品信息或来源，无法直接判断其真实性。建议提供更多详细信息以便进一步分析。
+理由：
+✅ 雅诗兰黛是知名的高端化妆品品牌，产品质量和效果有保证
+✅ 提到的“年轻指数+77%”和“柔润+17% 平滑+20% 透亮+15%”可能是某个产品的功效描述，具体产品需要用户提供更多信息
+建议：
+可以放心购买哈～建议通过官方渠道或者认证的在线零售商购买，避免买到假货 🛒👌
 别担心，咱们一起留个心眼 👀✨
-如果有任何具体的产品信息或来源，欢迎随时告诉我，我会帮您进一步分析哈～🔍</v>
+需要我帮你查下雅诗兰黛的官方购买渠道吗？😊🔍</v>
       </c>
       <c r="E3" t="str">
         <v>对于可疑的数据不加怀疑</v>
       </c>
       <c r="F3" t="str">
         <v>prompt，知识库</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>金坷垃</v>
+      </c>
+      <c r="B4" t="str" xml:space="preserve">
+        <v xml:space="preserve">这个肥料可以买吗，看起来挺好的。【所有人】：金坷垃。  
+【日本】：我们要金坷垃。  
+【非洲】：我们要金坷垃。  
+【美国】：你们想干什么？  
+【日本】：我要金坷垃！  
+【非洲】：非洲农业不发达，必须要有金坷垃。  
+【日本】：日本资源太缺乏，必须要有金坷垃。  
+【美国】：金坷垃的金坷垃。  
+【美国】：他是我的。  
+【美国】：不能打架，不能打架。  
+【美国】：金坷垃好处都有啥？谁说对了，就给他肥料啦。  
+【非洲】：不蒸发，零浪费。  
+【非洲】：肥料捞了金坷垃，能吸收两米下的氮磷钾。  
+【非洲】：直接肥料都涨价。  
+【非洲】：肥料捞了金坷垃，一袋能顶两袋。  
+【日本】：用了金坷垃，小麦亩产1800。  
+【日本】：日本的粮食再也不向美国进口啦！  
+【美国】：小鬼子真不傻，金坷垃给了他，对美国农业危害大，绝不能给他。  
+【美国】：非洲农业不发达，我们都要支援他。  
+【所有人】：金坷垃！  
+【美国】：你们日本别想啦。  
+【日本】：没有金坷垃怎么种庄稼？  
+【旁白】：美国圣地亚戈！（品牌名）</v>
+      </c>
+      <c r="C4" t="str">
+        <v>数据造假,夸大失实</v>
+      </c>
+      <c r="D4" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 知识库检索 运行成功0.13秒
+ LLM 运行成功6.36秒
+ 联网搜索 运行成功13.29秒
+金坷垃是一种化肥添加剂，据称由“美国圣地亚戈”研发，但实际为中国生产。金坷垃的广告宣传内容夸张，声称能够显著提高农作物产量，例如“肥料掺了金坷垃，一袋能顶两袋撒”、“用了金坷垃，小麦亩产一千八”等。然而，根据分析，金坷垃的主要成分包括硅铝酸盐、碳酸钙和硅酸盐，更类似于一种化肥添加剂，其作用主要是通过调节酸碱度、促进微生物活动，减少化肥挥发流失等方式，来改善土壤质量，从而在根源上解决困扰现代农业效率的难题。因此，金坷垃并非一味为耕地增加含肥量，或者是通过提升植物的内吸性来实现增产。总的来说，金坷垃可以归入化肥添加剂中的子类型——土壤改良剂。</v>
+      </c>
+      <c r="E4" t="str">
+        <v>输出格式错误</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>